<commit_message>
files modified for paper
</commit_message>
<xml_diff>
--- a/2_DA_Accuracy_Experiments/Saved_Models/Compiled Accuracy.xlsx
+++ b/2_DA_Accuracy_Experiments/Saved_Models/Compiled Accuracy.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/42632c7fcf3d8c0e/Desktop/MIDS_Courses/Spring_2022/w266-project-Dera-Evan-Kieran/2_DA_Accuracy_Experiments/Saved_Models/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="160" documentId="11_F25DC773A252ABDACC1048A471DE5A765BDE58EA" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{76FD9E23-C6BE-440B-A8AF-ADB7999B354E}"/>
+  <xr:revisionPtr revIDLastSave="283" documentId="11_F25DC773A252ABDACC1048A471DE5A765BDE58EA" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1F72E8F3-F9F8-4C3C-BB00-45CC32D1769F}"/>
   <bookViews>
-    <workbookView xWindow="3510" yWindow="3510" windowWidth="57600" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="23475" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="All Model Metrics" sheetId="2" r:id="rId1"/>
+    <sheet name="Accuracy Only" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="38">
   <si>
     <t>Trial Name</t>
   </si>
@@ -118,15 +119,46 @@
     <t>x8</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
+    <t>Augmented SR 0.7</t>
+  </si>
+  <si>
+    <t>Augmented RI 0.7</t>
+  </si>
+  <si>
+    <t>Augmented RS 0.7</t>
+  </si>
+  <si>
+    <t>Augmented RD 0.7</t>
+  </si>
+  <si>
+    <t>5 Augmentations</t>
+  </si>
+  <si>
+    <t>Training Examples</t>
+  </si>
+  <si>
+    <t>2 Augmentations</t>
+  </si>
+  <si>
+    <t>7 Augmentations</t>
+  </si>
+  <si>
+    <t>10 Augmentations</t>
+  </si>
+  <si>
+    <t>Aug Contextual Ins</t>
+  </si>
+  <si>
+    <t>Aug Contextual Sub</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="170" formatCode="0.00000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -157,7 +189,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -170,6 +202,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -212,7 +248,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$17</c:f>
+              <c:f>'Accuracy Only'!$B$17</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -235,7 +271,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$C$16:$G$16</c:f>
+              <c:f>'Accuracy Only'!$C$16:$G$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -259,12 +295,12 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$17:$G$17</c:f>
+              <c:f>'Accuracy Only'!$C$17:$G$17</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>0.68694747789911503</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.706708</c:v>
@@ -293,7 +329,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$18</c:f>
+              <c:f>'Accuracy Only'!$B$18</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -316,7 +352,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$C$16:$G$16</c:f>
+              <c:f>'Accuracy Only'!$C$16:$G$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -340,7 +376,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$18:$G$18</c:f>
+              <c:f>'Accuracy Only'!$C$18:$G$18</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="5"/>
@@ -374,7 +410,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$19</c:f>
+              <c:f>'Accuracy Only'!$B$19</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -397,7 +433,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$C$16:$G$16</c:f>
+              <c:f>'Accuracy Only'!$C$16:$G$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -421,7 +457,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$19:$G$19</c:f>
+              <c:f>'Accuracy Only'!$C$19:$G$19</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="5"/>
@@ -455,7 +491,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$20</c:f>
+              <c:f>'Accuracy Only'!$B$20</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -478,7 +514,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$C$16:$G$16</c:f>
+              <c:f>'Accuracy Only'!$C$16:$G$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -502,7 +538,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$20:$G$20</c:f>
+              <c:f>'Accuracy Only'!$C$20:$G$20</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="5"/>
@@ -536,7 +572,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$21</c:f>
+              <c:f>'Accuracy Only'!$B$21</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -559,7 +595,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$C$16:$G$16</c:f>
+              <c:f>'Accuracy Only'!$C$16:$G$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -583,7 +619,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$21:$G$21</c:f>
+              <c:f>'Accuracy Only'!$C$21:$G$21</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="5"/>
@@ -617,7 +653,7 @@
           <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$22</c:f>
+              <c:f>'Accuracy Only'!$B$22</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -640,7 +676,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$C$16:$G$16</c:f>
+              <c:f>'Accuracy Only'!$C$16:$G$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -664,7 +700,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$22:$G$22</c:f>
+              <c:f>'Accuracy Only'!$C$22:$G$22</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="5"/>
@@ -698,7 +734,7 @@
           <c:order val="6"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$23</c:f>
+              <c:f>'Accuracy Only'!$B$23</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -723,7 +759,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$C$16:$G$16</c:f>
+              <c:f>'Accuracy Only'!$C$16:$G$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -747,7 +783,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$23:$G$23</c:f>
+              <c:f>'Accuracy Only'!$C$23:$G$23</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="5"/>
@@ -781,7 +817,7 @@
           <c:order val="7"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$24</c:f>
+              <c:f>'Accuracy Only'!$B$24</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -806,7 +842,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$C$16:$G$16</c:f>
+              <c:f>'Accuracy Only'!$C$16:$G$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -830,7 +866,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$24:$G$24</c:f>
+              <c:f>'Accuracy Only'!$C$24:$G$24</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="5"/>
@@ -1212,7 +1248,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$17</c:f>
+              <c:f>'Accuracy Only'!$B$17</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1233,7 +1269,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$16:$G$16</c:f>
+              <c:f>'Accuracy Only'!$C$16:$G$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -1257,12 +1293,12 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$17:$G$17</c:f>
+              <c:f>'Accuracy Only'!$C$17:$G$17</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>0.68694747789911503</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.706708</c:v>
@@ -1290,7 +1326,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$18</c:f>
+              <c:f>'Accuracy Only'!$B$18</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1311,7 +1347,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$16:$G$16</c:f>
+              <c:f>'Accuracy Only'!$C$16:$G$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -1335,7 +1371,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$18:$G$18</c:f>
+              <c:f>'Accuracy Only'!$C$18:$G$18</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="5"/>
@@ -1368,7 +1404,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$19</c:f>
+              <c:f>'Accuracy Only'!$B$19</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1389,7 +1425,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$16:$G$16</c:f>
+              <c:f>'Accuracy Only'!$C$16:$G$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -1413,7 +1449,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$19:$G$19</c:f>
+              <c:f>'Accuracy Only'!$C$19:$G$19</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="5"/>
@@ -1446,7 +1482,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$20</c:f>
+              <c:f>'Accuracy Only'!$B$20</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1467,7 +1503,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$16:$G$16</c:f>
+              <c:f>'Accuracy Only'!$C$16:$G$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -1491,7 +1527,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$20:$G$20</c:f>
+              <c:f>'Accuracy Only'!$C$20:$G$20</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="5"/>
@@ -1524,7 +1560,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$21</c:f>
+              <c:f>'Accuracy Only'!$B$21</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1545,7 +1581,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$16:$G$16</c:f>
+              <c:f>'Accuracy Only'!$C$16:$G$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -1569,7 +1605,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$21:$G$21</c:f>
+              <c:f>'Accuracy Only'!$C$21:$G$21</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="5"/>
@@ -1602,7 +1638,7 @@
           <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$22</c:f>
+              <c:f>'Accuracy Only'!$B$22</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1623,7 +1659,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$16:$G$16</c:f>
+              <c:f>'Accuracy Only'!$C$16:$G$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -1647,7 +1683,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$22:$G$22</c:f>
+              <c:f>'Accuracy Only'!$C$22:$G$22</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="5"/>
@@ -1680,7 +1716,7 @@
           <c:order val="6"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$23</c:f>
+              <c:f>'Accuracy Only'!$B$23</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1703,7 +1739,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$16:$G$16</c:f>
+              <c:f>'Accuracy Only'!$C$16:$G$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -1727,7 +1763,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$23:$G$23</c:f>
+              <c:f>'Accuracy Only'!$C$23:$G$23</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="5"/>
@@ -1760,7 +1796,7 @@
           <c:order val="7"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$24</c:f>
+              <c:f>'Accuracy Only'!$B$24</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1783,7 +1819,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$16:$G$16</c:f>
+              <c:f>'Accuracy Only'!$C$16:$G$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -1807,7 +1843,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$24:$G$24</c:f>
+              <c:f>'Accuracy Only'!$C$24:$G$24</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="5"/>
@@ -3619,11 +3655,598 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCB91E52-FECD-4186-BEB2-826A21ED7CB0}">
+  <dimension ref="A1:P23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I23" sqref="I23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="17.5703125" customWidth="1"/>
+    <col min="8" max="8" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="18.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B1" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="L1" s="6"/>
+      <c r="M1" s="6"/>
+      <c r="N1" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="O1" s="6"/>
+      <c r="P1" s="6"/>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="6">
+        <v>15383</v>
+      </c>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6">
+        <v>46149</v>
+      </c>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6">
+        <v>92298</v>
+      </c>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6">
+        <v>123064</v>
+      </c>
+      <c r="L2" s="6"/>
+      <c r="M2" s="6"/>
+      <c r="N2" s="6">
+        <v>169213</v>
+      </c>
+      <c r="O2" s="6"/>
+      <c r="P2" s="6"/>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H3" t="s">
+        <v>1</v>
+      </c>
+      <c r="I3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J3" t="s">
+        <v>3</v>
+      </c>
+      <c r="K3" t="s">
+        <v>1</v>
+      </c>
+      <c r="L3" t="s">
+        <v>2</v>
+      </c>
+      <c r="M3" t="s">
+        <v>3</v>
+      </c>
+      <c r="N3" t="s">
+        <v>1</v>
+      </c>
+      <c r="O3" t="s">
+        <v>2</v>
+      </c>
+      <c r="P3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="7">
+        <v>0.68694747789911503</v>
+      </c>
+      <c r="C4" s="7">
+        <v>0.67158065676012302</v>
+      </c>
+      <c r="D4" s="7">
+        <v>0.75646636438304904</v>
+      </c>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="7"/>
+      <c r="L4" s="7"/>
+      <c r="M4" s="7"/>
+      <c r="N4" s="7"/>
+      <c r="O4" s="7"/>
+      <c r="P4" s="7"/>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7">
+        <v>0.70670826833073297</v>
+      </c>
+      <c r="F5" s="7">
+        <v>0.69063258531814697</v>
+      </c>
+      <c r="G5" s="7">
+        <v>0.77154031661293099</v>
+      </c>
+      <c r="H5" s="7">
+        <v>0.70306812272490904</v>
+      </c>
+      <c r="I5" s="7">
+        <v>0.68001776673618597</v>
+      </c>
+      <c r="J5" s="7">
+        <v>0.76577796822920696</v>
+      </c>
+      <c r="K5" s="7">
+        <v>0.69318772750909996</v>
+      </c>
+      <c r="L5" s="7">
+        <v>0.67491584574556995</v>
+      </c>
+      <c r="M5" s="7">
+        <v>0.76138704523575595</v>
+      </c>
+      <c r="N5" s="7">
+        <v>0.70358814352574095</v>
+      </c>
+      <c r="O5" s="7">
+        <v>0.67880505538153801</v>
+      </c>
+      <c r="P5" s="7">
+        <v>0.76402279908485804</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7">
+        <v>0.70670826833073297</v>
+      </c>
+      <c r="F6" s="7">
+        <v>0.67894491486879405</v>
+      </c>
+      <c r="G6" s="7">
+        <v>0.76637824299281698</v>
+      </c>
+      <c r="H6" s="7">
+        <v>0.69734789391575602</v>
+      </c>
+      <c r="I6" s="7">
+        <v>0.67086438846952001</v>
+      </c>
+      <c r="J6" s="7">
+        <v>0.75992479762395704</v>
+      </c>
+      <c r="K6" s="7">
+        <v>0.70670826833073297</v>
+      </c>
+      <c r="L6" s="7">
+        <v>0.68703323753407297</v>
+      </c>
+      <c r="M6" s="7">
+        <v>0.77093471539381697</v>
+      </c>
+      <c r="N6" s="7">
+        <v>0.70098803952157995</v>
+      </c>
+      <c r="O6" s="7">
+        <v>0.68466916772969799</v>
+      </c>
+      <c r="P6" s="7">
+        <v>0.76832414017888195</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7">
+        <v>0.702028081123244</v>
+      </c>
+      <c r="F7" s="7">
+        <v>0.68253067364683895</v>
+      </c>
+      <c r="G7" s="7">
+        <v>0.76724178639791596</v>
+      </c>
+      <c r="H7" s="7">
+        <v>0.71346853874154903</v>
+      </c>
+      <c r="I7" s="7">
+        <v>0.69612523629908096</v>
+      </c>
+      <c r="J7" s="7">
+        <v>0.77792720640453294</v>
+      </c>
+      <c r="K7" s="7">
+        <v>0.70670826833073297</v>
+      </c>
+      <c r="L7" s="7">
+        <v>0.68181793074583197</v>
+      </c>
+      <c r="M7" s="7">
+        <v>0.76893756384581102</v>
+      </c>
+      <c r="N7" s="7">
+        <v>0.71086843473738903</v>
+      </c>
+      <c r="O7" s="7">
+        <v>0.69186439998653404</v>
+      </c>
+      <c r="P7" s="7">
+        <v>0.77396867714002304</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7">
+        <v>0.70410816432657297</v>
+      </c>
+      <c r="F8" s="7">
+        <v>0.68522212235851498</v>
+      </c>
+      <c r="G8" s="7">
+        <v>0.76774752458185802</v>
+      </c>
+      <c r="H8" s="7">
+        <v>0.70098803952157995</v>
+      </c>
+      <c r="I8" s="7">
+        <v>0.68376272631729296</v>
+      </c>
+      <c r="J8" s="7">
+        <v>0.76599708714586801</v>
+      </c>
+      <c r="K8" s="7">
+        <v>0.71190847633905296</v>
+      </c>
+      <c r="L8" s="7">
+        <v>0.68749724779890198</v>
+      </c>
+      <c r="M8" s="7">
+        <v>0.77207875484065602</v>
+      </c>
+      <c r="N8" s="7">
+        <v>0.69370774830993198</v>
+      </c>
+      <c r="O8" s="7">
+        <v>0.67247983277120404</v>
+      </c>
+      <c r="P8" s="7">
+        <v>0.76003185331874701</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7">
+        <v>0.70046801872074804</v>
+      </c>
+      <c r="F9" s="7">
+        <v>0.68009895850797597</v>
+      </c>
+      <c r="G9" s="7">
+        <v>0.76555144385378504</v>
+      </c>
+      <c r="H9" s="7">
+        <v>0.70098803952157995</v>
+      </c>
+      <c r="I9" s="7">
+        <v>0.67193465183448697</v>
+      </c>
+      <c r="J9" s="7">
+        <v>0.76202786338430095</v>
+      </c>
+      <c r="K9" s="7">
+        <v>0.70306812272490904</v>
+      </c>
+      <c r="L9" s="7">
+        <v>0.68808210191171804</v>
+      </c>
+      <c r="M9" s="7">
+        <v>0.77158808181918204</v>
+      </c>
+      <c r="N9" s="7">
+        <v>0.69994799791991602</v>
+      </c>
+      <c r="O9" s="7">
+        <v>0.681153024477542</v>
+      </c>
+      <c r="P9" s="7">
+        <v>0.76654184335991005</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7">
+        <v>0.70930837233489297</v>
+      </c>
+      <c r="F10" s="7">
+        <v>0.68869701964729602</v>
+      </c>
+      <c r="G10" s="7">
+        <v>0.77017428514412101</v>
+      </c>
+      <c r="H10" s="7">
+        <v>0.702028081123244</v>
+      </c>
+      <c r="I10" s="7">
+        <v>0.674501774971489</v>
+      </c>
+      <c r="J10" s="7">
+        <v>0.76553081248808497</v>
+      </c>
+      <c r="K10" s="7">
+        <v>0.70618824752990095</v>
+      </c>
+      <c r="L10" s="7">
+        <v>0.68091574308604697</v>
+      </c>
+      <c r="M10" s="7">
+        <v>0.76681616756842197</v>
+      </c>
+      <c r="N10" s="7">
+        <v>0.69838793551741996</v>
+      </c>
+      <c r="O10" s="7">
+        <v>0.67870706405325698</v>
+      </c>
+      <c r="P10" s="7">
+        <v>0.76333132742173604</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>36</v>
+      </c>
+      <c r="E11" s="7">
+        <v>0.71034841393655701</v>
+      </c>
+      <c r="F11" s="7">
+        <v>0.68821065863695896</v>
+      </c>
+      <c r="G11" s="7">
+        <v>0.77136618987074301</v>
+      </c>
+      <c r="H11" s="7">
+        <v>0.69786791471658804</v>
+      </c>
+      <c r="I11" s="7">
+        <v>0.67550444910448004</v>
+      </c>
+      <c r="J11" s="7">
+        <v>0.77069393703393596</v>
+      </c>
+      <c r="K11" s="7">
+        <v>0.69318772750909996</v>
+      </c>
+      <c r="L11" s="7">
+        <v>0.67724163232511503</v>
+      </c>
+      <c r="M11" s="7">
+        <v>0.76135864573770495</v>
+      </c>
+      <c r="N11" s="7">
+        <v>0.68486739469578695</v>
+      </c>
+      <c r="O11" s="7">
+        <v>0.66763271387692102</v>
+      </c>
+      <c r="P11" s="7">
+        <v>0.75375931782384697</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>37</v>
+      </c>
+      <c r="E12" s="7">
+        <v>0.69734789391575602</v>
+      </c>
+      <c r="F12" s="7">
+        <v>0.67361434655136998</v>
+      </c>
+      <c r="G12" s="7">
+        <v>0.76181647413155495</v>
+      </c>
+      <c r="H12" s="7">
+        <v>0.70826833073322903</v>
+      </c>
+      <c r="I12" s="7">
+        <v>0.68198721018273001</v>
+      </c>
+      <c r="J12" s="7">
+        <v>0.77532357705929</v>
+      </c>
+      <c r="K12" s="7">
+        <v>0.696827873114924</v>
+      </c>
+      <c r="L12" s="7">
+        <v>0.68065140413871295</v>
+      </c>
+      <c r="M12" s="7">
+        <v>0.76731399760279095</v>
+      </c>
+      <c r="N12" s="7">
+        <v>0.69006760270410805</v>
+      </c>
+      <c r="O12" s="7">
+        <v>0.67836048854720599</v>
+      </c>
+      <c r="P12" s="7">
+        <v>0.76261262499347504</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="H14" s="7"/>
+      <c r="L14" s="4"/>
+      <c r="M14" s="4"/>
+      <c r="N14" s="4"/>
+      <c r="O14" s="4"/>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="H15" s="7"/>
+      <c r="I15" s="7"/>
+      <c r="J15" s="7"/>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="H16" s="7"/>
+      <c r="I16" s="7"/>
+      <c r="J16" s="7"/>
+      <c r="K16" s="2"/>
+      <c r="L16" s="2"/>
+      <c r="M16" s="2"/>
+      <c r="N16" s="5"/>
+      <c r="O16" s="2"/>
+    </row>
+    <row r="17" spans="11:15" x14ac:dyDescent="0.25">
+      <c r="K17" s="2"/>
+      <c r="L17" s="2"/>
+      <c r="M17" s="2"/>
+      <c r="N17" s="5"/>
+      <c r="O17" s="2"/>
+    </row>
+    <row r="18" spans="11:15" x14ac:dyDescent="0.25">
+      <c r="K18" s="2"/>
+      <c r="L18" s="2"/>
+      <c r="M18" s="2"/>
+      <c r="N18" s="5"/>
+      <c r="O18" s="2"/>
+    </row>
+    <row r="19" spans="11:15" x14ac:dyDescent="0.25">
+      <c r="K19" s="2"/>
+      <c r="L19" s="2"/>
+      <c r="M19" s="2"/>
+      <c r="N19" s="5"/>
+      <c r="O19" s="2"/>
+    </row>
+    <row r="20" spans="11:15" x14ac:dyDescent="0.25">
+      <c r="K20" s="2"/>
+      <c r="L20" s="2"/>
+      <c r="M20" s="2"/>
+      <c r="N20" s="5"/>
+      <c r="O20" s="2"/>
+    </row>
+    <row r="21" spans="11:15" x14ac:dyDescent="0.25">
+      <c r="K21" s="2"/>
+      <c r="L21" s="2"/>
+      <c r="M21" s="2"/>
+      <c r="N21" s="5"/>
+      <c r="O21" s="2"/>
+    </row>
+    <row r="22" spans="11:15" x14ac:dyDescent="0.25">
+      <c r="K22" s="2"/>
+      <c r="L22" s="2"/>
+      <c r="M22" s="2"/>
+      <c r="N22" s="5"/>
+      <c r="O22" s="2"/>
+    </row>
+    <row r="23" spans="11:15" x14ac:dyDescent="0.25">
+      <c r="K23" s="2"/>
+      <c r="L23" s="2"/>
+      <c r="M23" s="2"/>
+      <c r="N23" s="5"/>
+      <c r="O23" s="2"/>
+    </row>
+  </sheetData>
+  <mergeCells count="10">
+    <mergeCell ref="K1:M1"/>
+    <mergeCell ref="K2:M2"/>
+    <mergeCell ref="N1:P1"/>
+    <mergeCell ref="N2:P2"/>
+    <mergeCell ref="H1:J1"/>
+    <mergeCell ref="H2:J2"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="B1:D1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17:C24"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23:E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3885,13 +4508,13 @@
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="C14" s="4" t="s">
+      <c r="C14" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C15" t="s">
@@ -3935,8 +4558,8 @@
       <c r="B17" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="2" t="s">
-        <v>27</v>
+      <c r="C17" s="2">
+        <v>0.68694747789911503</v>
       </c>
       <c r="D17" s="2">
         <v>0.706708</v>

</xml_diff>